<commit_message>
adding baiama rodents from ODK and manually adding 5 missing rodents
</commit_message>
<xml_diff>
--- a/data/missing_grids.xlsx
+++ b/data/missing_grids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ucbtds4\R_Repositories\rodent_trapping\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8410EB71-D1CE-4E7D-AC64-E9EA4B41E15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E30664B-8129-4243-9E82-D3D88EA99C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13716" yWindow="0" windowWidth="8904" windowHeight="12084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
   <si>
     <t>village</t>
   </si>
@@ -369,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,10 +441,10 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="E4">
         <v>49</v>
@@ -452,16 +452,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>50</v>
+        <v>148</v>
       </c>
       <c r="E5">
         <v>49</v>
@@ -469,16 +469,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
       <c r="D6">
-        <v>99</v>
+        <v>197</v>
       </c>
       <c r="E6">
         <v>49</v>
@@ -486,16 +486,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="E7">
         <v>49</v>
@@ -503,19 +503,19 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>197</v>
+        <v>148</v>
       </c>
       <c r="E8">
-        <v>97</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -523,13 +523,13 @@
         <v>6</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>148</v>
+        <v>197</v>
       </c>
       <c r="E9">
         <v>49</v>
@@ -537,13 +537,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
         <v>6</v>
       </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
       <c r="C10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D10">
         <v>197</v>
@@ -554,16 +554,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>8</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>49</v>
@@ -571,16 +571,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B12">
         <v>8</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>148</v>
+        <v>50</v>
       </c>
       <c r="E12">
         <v>49</v>
@@ -588,16 +588,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B13">
         <v>8</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D13">
-        <v>197</v>
+        <v>99</v>
       </c>
       <c r="E13">
         <v>49</v>
@@ -611,10 +611,10 @@
         <v>8</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>148</v>
       </c>
       <c r="E14">
         <v>49</v>
@@ -628,10 +628,10 @@
         <v>8</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D15">
-        <v>50</v>
+        <v>246</v>
       </c>
       <c r="E15">
         <v>49</v>
@@ -639,86 +639,18 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B16">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>99</v>
+        <v>197</v>
       </c>
       <c r="E16">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17">
-        <v>8</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="D17">
-        <v>148</v>
-      </c>
-      <c r="E17">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18">
-        <v>8</v>
-      </c>
-      <c r="C18">
-        <v>7</v>
-      </c>
-      <c r="D18">
-        <v>246</v>
-      </c>
-      <c r="E18">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19">
-        <v>9</v>
-      </c>
-      <c r="C19">
-        <v>7</v>
-      </c>
-      <c r="D19">
-        <v>197</v>
-      </c>
-      <c r="E19">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20">
-        <v>4</v>
-      </c>
-      <c r="C20">
-        <v>5</v>
-      </c>
-      <c r="D20">
-        <v>197</v>
-      </c>
-      <c r="E20">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final update for thesis data, can be updated as more sequencing becomes available but for now the data is final
</commit_message>
<xml_diff>
--- a/data/missing_grids.xlsx
+++ b/data/missing_grids.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ucbtds4\R_Repositories\rodent_trapping\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E30664B-8129-4243-9E82-D3D88EA99C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C6FE52-C979-4808-A080-FB6A0A840485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="9">
   <si>
     <t>village</t>
   </si>
@@ -369,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,6 +654,380 @@
         <v>49</v>
       </c>
     </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>50</v>
+      </c>
+      <c r="E18">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>99</v>
+      </c>
+      <c r="E19">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>148</v>
+      </c>
+      <c r="E20">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>197</v>
+      </c>
+      <c r="E21">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>50</v>
+      </c>
+      <c r="E23">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>99</v>
+      </c>
+      <c r="E24">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>147</v>
+      </c>
+      <c r="E25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>197</v>
+      </c>
+      <c r="E26">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <v>246</v>
+      </c>
+      <c r="E27">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>50</v>
+      </c>
+      <c r="E29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>99</v>
+      </c>
+      <c r="E30">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <v>148</v>
+      </c>
+      <c r="E31">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>7</v>
+      </c>
+      <c r="D32">
+        <v>197</v>
+      </c>
+      <c r="E32">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>50</v>
+      </c>
+      <c r="E34">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>99</v>
+      </c>
+      <c r="E35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>148</v>
+      </c>
+      <c r="E36">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37">
+        <v>10</v>
+      </c>
+      <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>197</v>
+      </c>
+      <c r="E37">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38">
+        <v>246</v>
+      </c>
+      <c r="E38">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix some mildly off coords
</commit_message>
<xml_diff>
--- a/data/missing_grids.xlsx
+++ b/data/missing_grids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ucbtds4\R_Repositories\rodent_trapping\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C6FE52-C979-4808-A080-FB6A0A840485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4654C172-F41D-4C8B-AA39-3C5F06191F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,7 +372,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -801,7 +801,7 @@
         <v>4</v>
       </c>
       <c r="D25">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E25">
         <v>49</v>

</xml_diff>